<commit_message>
Update to version 0.1.2 with C14 dates as numeric
</commit_message>
<xml_diff>
--- a/notes/issues_notes.xlsx
+++ b/notes/issues_notes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t xml:space="preserve">Field/Category</t>
   </si>
@@ -64,6 +64,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Missing or Unknown (</t>
     </r>
@@ -73,6 +74,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不明</t>
     </r>
@@ -82,6 +84,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -113,6 +116,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">おなじ試料番号を持つエントリーの「試料コード</t>
     </r>
@@ -121,6 +125,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -129,6 +134,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">」が違う。 </t>
     </r>
@@ -142,6 +148,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">おなじ試料番号を持つエントリーの「試料コード</t>
     </r>
@@ -150,6 +157,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -158,6 +166,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">」が違う。 </t>
     </r>
@@ -174,6 +183,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">おなじ試料番号を持つエントリーの「</t>
     </r>
@@ -182,6 +192,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14C</t>
     </r>
@@ -190,6 +201,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年代」が違う。 </t>
     </r>
@@ -209,6 +221,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">「</t>
     </r>
@@ -217,6 +230,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14C</t>
     </r>
@@ -225,6 +239,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年代（</t>
     </r>
@@ -233,6 +248,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Conventional 14C age)</t>
     </r>
@@ -241,6 +257,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">」もしくは「暦年較正用</t>
     </r>
@@ -249,6 +266,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14C</t>
     </r>
@@ -257,6 +275,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年代」に数字以外の文字が記入されている。</t>
     </r>
@@ -273,6 +292,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">「</t>
     </r>
@@ -281,6 +301,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14C</t>
     </r>
@@ -289,6 +310,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年代（</t>
     </r>
@@ -297,6 +319,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Conventional 14C age)</t>
     </r>
@@ -305,6 +328,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">」と「暦年較正用</t>
     </r>
@@ -313,6 +337,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">14C</t>
     </r>
@@ -321,6 +346,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">年代」の誤差が５０年以上である。</t>
     </r>
@@ -355,6 +381,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">「遺跡名」は同じだが「緯度」・「経度」は異なる。</t>
     </r>
@@ -363,6 +390,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dist</t>
     </r>
@@ -371,6 +399,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">は遺跡間の距離</t>
     </r>
@@ -390,6 +419,7 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">「遺跡名」の字が違っている可能性がある。</t>
     </r>
@@ -398,6 +428,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">XXX</t>
     </r>
@@ -406,12 +437,19 @@
         <sz val="10"/>
         <rFont val="Source Han Sans CN"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">は訂正</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">報告書をチェックしてから訂正</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site Name missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">「遺跡名」が記録されていない</t>
   </si>
 </sst>
 </file>
@@ -421,11 +459,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -447,32 +486,43 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Source Han Sans CN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Source Han Sans CN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Source Han Sans CN"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
+      <sz val="10"/>
+      <name val="Source Han Sans CN"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Source Han Sans CN"/>
       <family val="2"/>
@@ -641,7 +691,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -760,6 +810,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -839,13 +893,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ18"/>
+  <dimension ref="A1:AMJ19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.42"/>
@@ -1047,7 +1101,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="30.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="s">
         <v>43</v>
       </c>
@@ -1061,14 +1115,27 @@
         <v>46</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="30.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A2:A12"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="D6:D12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>